<commit_message>
added linearization to graph
</commit_message>
<xml_diff>
--- a/experiments/SensorGraph.xlsx
+++ b/experiments/SensorGraph.xlsx
@@ -219,6 +219,21 @@
           <c:tx>
             <c:v>Right Sensor</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0797913618098623"/>
+                  <c:y val="0.018790097183798"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Sensor Readings'!$S$3:$S$322</c:f>
@@ -425,6 +440,21 @@
           <c:tx>
             <c:v>Left Sensor</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0701631709753095"/>
+                  <c:y val="0.0309894303752571"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Sensor Readings'!$S$3:$S$322</c:f>
@@ -631,6 +661,21 @@
           <c:tx>
             <c:v>Right Center Sensor</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.249912549648108"/>
+                  <c:y val="-0.220794920905157"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Sensor Readings'!$S$3:$S$322</c:f>
@@ -837,6 +882,21 @@
           <c:tx>
             <c:v>Left Center Sensor</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.118113197686572"/>
+                  <c:y val="-0.105774420089381"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Sensor Readings'!$S$3:$S$322</c:f>
@@ -1458,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W332"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V338" sqref="V338"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B3" activeCellId="1" sqref="A3:A322 B3:B322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updated graph for 1 sensor
</commit_message>
<xml_diff>
--- a/experiments/SensorGraph.xlsx
+++ b/experiments/SensorGraph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sensor Readings" sheetId="1" r:id="rId1"/>
@@ -147,12 +147,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -160,6 +154,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -216,6 +216,480 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.103448275862069"/>
+                  <c:y val="-0.290476917129545"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$G$3:$G$58</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$H$3:$H$58</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3620.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3455.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3003.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2523.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2165.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1914.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0706983946510996"/>
+                  <c:y val="-0.00921849885043439"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$G$58:$G$113</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$H$58:$H$113</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1914.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1748.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1612.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1511.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1412.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1348.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0824202416508281"/>
+                  <c:y val="-0.0591993733341472"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$G$113:$G$168</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$H$113:$H$168</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1348.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1290.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1239.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1200.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1167.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1137.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0112175875644855"/>
+                  <c:y val="0.0317328938533846"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$G$168:$G$223</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$H$168:$H$223</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1137.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1114.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1094.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1076.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1061.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1048.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0180597508824328"/>
+                  <c:y val="-0.0620273047264441"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$G$223:$G$322</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$H$223:$H$322</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1048.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1039.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1029.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1019.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1012.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1005.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>995.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>992.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>987.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2074606808"/>
+        <c:axId val="2074617768"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2074606808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0&quot; cm&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2074617768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2074617768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2074606808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:tx>
             <c:v>Right Sensor</c:v>
           </c:tx>
@@ -1105,11 +1579,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2131373784"/>
-        <c:axId val="2130196616"/>
+        <c:axId val="2052222360"/>
+        <c:axId val="2052219880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2131373784"/>
+        <c:axId val="2052222360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1119,12 +1593,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130196616"/>
+        <c:crossAx val="2052219880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2130196616"/>
+        <c:axId val="2052219880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,7 +1609,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131373784"/>
+        <c:crossAx val="2052222360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1158,6 +1632,41 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>333</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1518,93 +2027,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W332"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B3" activeCellId="1" sqref="A3:A322 B3:B322"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H3" activeCellId="1" sqref="G3:G58 H3:H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="G1" s="8" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="G1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="M1" s="8" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="M1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="S1" s="8" t="s">
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="S1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="5"/>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="9" t="s">
+      <c r="M2" s="6"/>
+      <c r="N2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="7"/>
-      <c r="T2" s="9" t="s">
+      <c r="S2" s="6"/>
+      <c r="T2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="U2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="V2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="W2" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1616,11 +2125,11 @@
         <f>AVERAGE(A4:A13)</f>
         <v>3641.4</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <f>STDEV(B4:B13)</f>
         <v>1.2292725943057186</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <f>MAX(B4:B13)-MIN(B4:B13)</f>
         <v>4</v>
       </c>
@@ -1635,11 +2144,11 @@
         <f>AVERAGE(G4:G13)</f>
         <v>3620.4</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <f>STDEV(H4:H13)</f>
         <v>1.7795130420052185</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="8">
         <f>MAX(H4:H13)-MIN(H4:H13)</f>
         <v>6</v>
       </c>
@@ -1654,11 +2163,11 @@
         <f>AVERAGE(M4:M13)</f>
         <v>3823.2</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="8">
         <f>STDEV(N4:N13)</f>
         <v>1.5670212364724214</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="8">
         <f>MAX(N4:N13)-MIN(N4:N13)</f>
         <v>6</v>
       </c>
@@ -1673,11 +2182,11 @@
         <f>AVERAGE(S4:S13)</f>
         <v>3860.2</v>
       </c>
-      <c r="U3" s="10">
+      <c r="U3" s="8">
         <f>STDEV(T4:T13)</f>
         <v>6.4195880795508309</v>
       </c>
-      <c r="V3" s="10">
+      <c r="V3" s="8">
         <f>MAX(T4:T13)-MIN(T4:T13)</f>
         <v>18</v>
       </c>
@@ -2044,11 +2553,11 @@
         <f>AVERAGE(A15:A24)</f>
         <v>3500</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="8">
         <f>STDEV(B15:B24)</f>
         <v>0.82327260234856459</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="8">
         <f>MAX(B15:B24)-MIN(B15:B24)</f>
         <v>3</v>
       </c>
@@ -2063,11 +2572,11 @@
         <f>AVERAGE(G15:G24)</f>
         <v>3455.5</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="8">
         <f>STDEV(H15:H24)</f>
         <v>0.91893658347268148</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="8">
         <f>MAX(H15:H24)-MIN(H15:H24)</f>
         <v>3</v>
       </c>
@@ -2082,11 +2591,11 @@
         <f>AVERAGE(M15:M24)</f>
         <v>3885.2</v>
       </c>
-      <c r="O14" s="10">
+      <c r="O14" s="8">
         <f>STDEV(N15:N24)</f>
         <v>0.99442892601175337</v>
       </c>
-      <c r="P14" s="10">
+      <c r="P14" s="8">
         <f>MAX(N15:N24)-MIN(N15:N24)</f>
         <v>3</v>
       </c>
@@ -2101,11 +2610,11 @@
         <f>AVERAGE(S15:S24)</f>
         <v>3884.1</v>
       </c>
-      <c r="U14" s="10">
+      <c r="U14" s="8">
         <f>STDEV(T15:T24)</f>
         <v>1.0327955589886446</v>
       </c>
-      <c r="V14" s="10">
+      <c r="V14" s="8">
         <f>MAX(T15:T24)-MIN(T15:T24)</f>
         <v>3</v>
       </c>
@@ -2472,11 +2981,11 @@
         <f>AVERAGE(A26:A35)</f>
         <v>3237.6</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="8">
         <f>STDEV(B26:B35)</f>
         <v>0.70710678118654757</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="8">
         <f>MAX(B26:B35)-MIN(B26:B35)</f>
         <v>2</v>
       </c>
@@ -2491,11 +3000,11 @@
         <f>AVERAGE(G26:G35)</f>
         <v>3003.8</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="8">
         <f>STDEV(H26:H35)</f>
         <v>0.87559503577091335</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="8">
         <f>MAX(H26:H35)-MIN(H26:H35)</f>
         <v>3</v>
       </c>
@@ -2510,11 +3019,11 @@
         <f>AVERAGE(M26:M35)</f>
         <v>3860.8</v>
       </c>
-      <c r="O25" s="10">
+      <c r="O25" s="8">
         <f>STDEV(N26:N35)</f>
         <v>1.3165611772087666</v>
       </c>
-      <c r="P25" s="10">
+      <c r="P25" s="8">
         <f>MAX(N26:N35)-MIN(N26:N35)</f>
         <v>5</v>
       </c>
@@ -2529,11 +3038,11 @@
         <f>AVERAGE(S26:S35)</f>
         <v>3843</v>
       </c>
-      <c r="U25" s="10">
+      <c r="U25" s="8">
         <f>STDEV(T26:T35)</f>
         <v>1.2866839377079189</v>
       </c>
-      <c r="V25" s="10">
+      <c r="V25" s="8">
         <f>MAX(T26:T35)-MIN(T26:T35)</f>
         <v>4</v>
       </c>
@@ -2900,11 +3409,11 @@
         <f>AVERAGE(A37:A46)</f>
         <v>2833.5</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="8">
         <f>STDEV(B37:B46)</f>
         <v>1.2866839377079189</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="8">
         <f>MAX(B37:B46)-MIN(B37:B46)</f>
         <v>4</v>
       </c>
@@ -2919,11 +3428,11 @@
         <f>AVERAGE(G37:G46)</f>
         <v>2523.9</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I36" s="8">
         <f>STDEV(H37:H46)</f>
         <v>1.1352924243950937</v>
       </c>
-      <c r="J36" s="10">
+      <c r="J36" s="8">
         <f>MAX(H37:H46)-MIN(H37:H46)</f>
         <v>4</v>
       </c>
@@ -2938,11 +3447,11 @@
         <f>AVERAGE(M37:M46)</f>
         <v>3818.2</v>
       </c>
-      <c r="O36" s="10">
+      <c r="O36" s="8">
         <f>STDEV(N37:N46)</f>
         <v>0.84327404271156781</v>
       </c>
-      <c r="P36" s="10">
+      <c r="P36" s="8">
         <f>MAX(N37:N46)-MIN(N37:N46)</f>
         <v>3</v>
       </c>
@@ -2957,11 +3466,11 @@
         <f>AVERAGE(S37:S46)</f>
         <v>3783.8</v>
       </c>
-      <c r="U36" s="10">
+      <c r="U36" s="8">
         <f>STDEV(T37:T46)</f>
         <v>1.699673171197595</v>
       </c>
-      <c r="V36" s="10">
+      <c r="V36" s="8">
         <f>MAX(T37:T46)-MIN(T37:T46)</f>
         <v>5</v>
       </c>
@@ -3328,11 +3837,11 @@
         <f>AVERAGE(A48:A57)</f>
         <v>2584.1999999999998</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="8">
         <f>STDEV(B48:B57)</f>
         <v>0.91893658347268148</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D47" s="8">
         <f>MAX(B48:B57)-MIN(B48:B57)</f>
         <v>3</v>
       </c>
@@ -3347,11 +3856,11 @@
         <f>AVERAGE(G48:G57)</f>
         <v>2165.1999999999998</v>
       </c>
-      <c r="I47" s="10">
+      <c r="I47" s="8">
         <f>STDEV(H48:H57)</f>
         <v>1.2649110640673518</v>
       </c>
-      <c r="J47" s="10">
+      <c r="J47" s="8">
         <f>MAX(H48:H57)-MIN(H48:H57)</f>
         <v>4</v>
       </c>
@@ -3366,11 +3875,11 @@
         <f>AVERAGE(M48:M57)</f>
         <v>3771.7</v>
       </c>
-      <c r="O47" s="10">
+      <c r="O47" s="8">
         <f>STDEV(N48:N57)</f>
         <v>1.1547005383792515</v>
       </c>
-      <c r="P47" s="10">
+      <c r="P47" s="8">
         <f>MAX(N48:N57)-MIN(N48:N57)</f>
         <v>4</v>
       </c>
@@ -3385,11 +3894,11 @@
         <f>AVERAGE(S48:S57)</f>
         <v>3663.7</v>
       </c>
-      <c r="U47" s="10">
+      <c r="U47" s="8">
         <f>STDEV(T48:T57)</f>
         <v>1.3703203194062976</v>
       </c>
-      <c r="V47" s="10">
+      <c r="V47" s="8">
         <f>MAX(T48:T57)-MIN(T48:T57)</f>
         <v>5</v>
       </c>
@@ -3756,11 +4265,11 @@
         <f>AVERAGE(A59:A68)</f>
         <v>2334.5</v>
       </c>
-      <c r="C58" s="10">
+      <c r="C58" s="8">
         <f>STDEV(B59:B68)</f>
         <v>0.91893658347268148</v>
       </c>
-      <c r="D58" s="10">
+      <c r="D58" s="8">
         <f>MAX(B59:B68)-MIN(B59:B68)</f>
         <v>3</v>
       </c>
@@ -3775,11 +4284,11 @@
         <f>AVERAGE(G59:G68)</f>
         <v>1914.5</v>
       </c>
-      <c r="I58" s="10">
+      <c r="I58" s="8">
         <f>STDEV(H59:H68)</f>
         <v>1.1352924243950935</v>
       </c>
-      <c r="J58" s="10">
+      <c r="J58" s="8">
         <f>MAX(H59:H68)-MIN(H59:H68)</f>
         <v>3</v>
       </c>
@@ -3794,11 +4303,11 @@
         <f>AVERAGE(M59:M68)</f>
         <v>3660.4</v>
       </c>
-      <c r="O58" s="10">
+      <c r="O58" s="8">
         <f>STDEV(N59:N68)</f>
         <v>1.2649110640673518</v>
       </c>
-      <c r="P58" s="10">
+      <c r="P58" s="8">
         <f>MAX(N59:N68)-MIN(N59:N68)</f>
         <v>5</v>
       </c>
@@ -3813,11 +4322,11 @@
         <f>AVERAGE(S59:S68)</f>
         <v>3492.7</v>
       </c>
-      <c r="U58" s="10">
+      <c r="U58" s="8">
         <f>STDEV(T59:T68)</f>
         <v>1.3498971154211057</v>
       </c>
-      <c r="V58" s="10">
+      <c r="V58" s="8">
         <f>MAX(T59:T68)-MIN(T59:T68)</f>
         <v>4</v>
       </c>
@@ -4184,11 +4693,11 @@
         <f>AVERAGE(A70:A79)</f>
         <v>2170.9</v>
       </c>
-      <c r="C69" s="10">
+      <c r="C69" s="8">
         <f>STDEV(B70:B79)</f>
         <v>1.7919573407620812</v>
       </c>
-      <c r="D69" s="10">
+      <c r="D69" s="8">
         <f>MAX(B70:B79)-MIN(B70:B79)</f>
         <v>7</v>
       </c>
@@ -4203,11 +4712,11 @@
         <f>AVERAGE(G70:G79)</f>
         <v>1748.5</v>
       </c>
-      <c r="I69" s="10">
+      <c r="I69" s="8">
         <f>STDEV(H70:H79)</f>
         <v>1.9578900207451218</v>
       </c>
-      <c r="J69" s="10">
+      <c r="J69" s="8">
         <f>MAX(H70:H79)-MIN(H70:H79)</f>
         <v>6</v>
       </c>
@@ -4222,11 +4731,11 @@
         <f>AVERAGE(M70:M79)</f>
         <v>3515.7</v>
       </c>
-      <c r="O69" s="10">
+      <c r="O69" s="8">
         <f>STDEV(N70:N79)</f>
         <v>2.7808871486152276</v>
       </c>
-      <c r="P69" s="10">
+      <c r="P69" s="8">
         <f>MAX(N70:N79)-MIN(N70:N79)</f>
         <v>9</v>
       </c>
@@ -4241,11 +4750,11 @@
         <f>AVERAGE(S70:S79)</f>
         <v>3212.8</v>
       </c>
-      <c r="U69" s="10">
+      <c r="U69" s="8">
         <f>STDEV(T70:T79)</f>
         <v>1.509230856356236</v>
       </c>
-      <c r="V69" s="10">
+      <c r="V69" s="8">
         <f>MAX(T70:T79)-MIN(T70:T79)</f>
         <v>5</v>
       </c>
@@ -4612,11 +5121,11 @@
         <f>AVERAGE(A81:A90)</f>
         <v>2041.6</v>
       </c>
-      <c r="C80" s="10">
+      <c r="C80" s="8">
         <f>STDEV(B81:B90)</f>
         <v>1.1547005383792515</v>
       </c>
-      <c r="D80" s="10">
+      <c r="D80" s="8">
         <f>MAX(B81:B90)-MIN(B81:B90)</f>
         <v>4</v>
       </c>
@@ -4631,11 +5140,11 @@
         <f>AVERAGE(G81:G90)</f>
         <v>1612.5</v>
       </c>
-      <c r="I80" s="10">
+      <c r="I80" s="8">
         <f>STDEV(H81:H90)</f>
         <v>1.1595018087284059</v>
       </c>
-      <c r="J80" s="10">
+      <c r="J80" s="8">
         <f>MAX(H81:H90)-MIN(H81:H90)</f>
         <v>4</v>
       </c>
@@ -4650,11 +5159,11 @@
         <f>AVERAGE(M81:M90)</f>
         <v>3285.2</v>
       </c>
-      <c r="O80" s="10">
+      <c r="O80" s="8">
         <f>STDEV(N81:N90)</f>
         <v>1.1972189997378648</v>
       </c>
-      <c r="P80" s="10">
+      <c r="P80" s="8">
         <f>MAX(N81:N90)-MIN(N81:N90)</f>
         <v>3</v>
       </c>
@@ -4669,11 +5178,11 @@
         <f>AVERAGE(S81:S90)</f>
         <v>2840.3</v>
       </c>
-      <c r="U80" s="10">
+      <c r="U80" s="8">
         <f>STDEV(T81:T90)</f>
         <v>1.3498971154211057</v>
       </c>
-      <c r="V80" s="10">
+      <c r="V80" s="8">
         <f>MAX(T81:T90)-MIN(T81:T90)</f>
         <v>5</v>
       </c>
@@ -5040,11 +5549,11 @@
         <f>AVERAGE(A92:A101)</f>
         <v>1951.3</v>
       </c>
-      <c r="C91" s="10">
+      <c r="C91" s="8">
         <f>STDEV(B92:B101)</f>
         <v>0.87559503577091324</v>
       </c>
-      <c r="D91" s="10">
+      <c r="D91" s="8">
         <f>MAX(B92:B101)-MIN(B92:B101)</f>
         <v>2</v>
       </c>
@@ -5059,11 +5568,11 @@
         <f>AVERAGE(G92:G101)</f>
         <v>1511.9</v>
       </c>
-      <c r="I91" s="10">
+      <c r="I91" s="8">
         <f>STDEV(H92:H101)</f>
         <v>0.82327260234856459</v>
       </c>
-      <c r="J91" s="10">
+      <c r="J91" s="8">
         <f>MAX(H92:H101)-MIN(H92:H101)</f>
         <v>3</v>
       </c>
@@ -5078,11 +5587,11 @@
         <f>AVERAGE(M92:M101)</f>
         <v>2995.7</v>
       </c>
-      <c r="O91" s="10">
+      <c r="O91" s="8">
         <f>STDEV(N92:N101)</f>
         <v>0.51639777949432231</v>
       </c>
-      <c r="P91" s="10">
+      <c r="P91" s="8">
         <f>MAX(N92:N101)-MIN(N92:N101)</f>
         <v>1</v>
       </c>
@@ -5097,11 +5606,11 @@
         <f>AVERAGE(S92:S101)</f>
         <v>2560.6999999999998</v>
       </c>
-      <c r="U91" s="10">
+      <c r="U91" s="8">
         <f>STDEV(T92:T101)</f>
         <v>1.8257418583505538</v>
       </c>
-      <c r="V91" s="10">
+      <c r="V91" s="8">
         <f>MAX(T92:T101)-MIN(T92:T101)</f>
         <v>5</v>
       </c>
@@ -5468,11 +5977,11 @@
         <f>AVERAGE(A103:A112)</f>
         <v>1879.6</v>
       </c>
-      <c r="C102" s="10">
+      <c r="C102" s="8">
         <f>STDEV(B103:B112)</f>
         <v>0.94868329805051377</v>
       </c>
-      <c r="D102" s="10">
+      <c r="D102" s="8">
         <f>MAX(B103:B112)-MIN(B103:B112)</f>
         <v>3</v>
       </c>
@@ -5487,11 +5996,11 @@
         <f>AVERAGE(G103:G112)</f>
         <v>1412.4</v>
       </c>
-      <c r="I102" s="10">
+      <c r="I102" s="8">
         <f>STDEV(H103:H112)</f>
         <v>0.84327404271156792</v>
       </c>
-      <c r="J102" s="10">
+      <c r="J102" s="8">
         <f>MAX(H103:H112)-MIN(H103:H112)</f>
         <v>3</v>
       </c>
@@ -5506,11 +6015,11 @@
         <f>AVERAGE(M103:M112)</f>
         <v>2718.2</v>
       </c>
-      <c r="O102" s="10">
+      <c r="O102" s="8">
         <f>STDEV(N103:N112)</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="P102" s="10">
+      <c r="P102" s="8">
         <f>MAX(N103:N112)-MIN(N103:N112)</f>
         <v>5</v>
       </c>
@@ -5525,11 +6034,11 @@
         <f>AVERAGE(S103:S112)</f>
         <v>2367.5</v>
       </c>
-      <c r="U102" s="10">
+      <c r="U102" s="8">
         <f>STDEV(T103:T112)</f>
         <v>0.69920589878010109</v>
       </c>
-      <c r="V102" s="10">
+      <c r="V102" s="8">
         <f>MAX(T103:T112)-MIN(T103:T112)</f>
         <v>2</v>
       </c>
@@ -5896,11 +6405,11 @@
         <f>AVERAGE(A114:A123)</f>
         <v>1823</v>
       </c>
-      <c r="C113" s="10">
+      <c r="C113" s="8">
         <f>STDEV(B114:B123)</f>
         <v>0.82327260234856459</v>
       </c>
-      <c r="D113" s="10">
+      <c r="D113" s="8">
         <f>MAX(B114:B123)-MIN(B114:B123)</f>
         <v>3</v>
       </c>
@@ -5915,11 +6424,11 @@
         <f>AVERAGE(G114:G123)</f>
         <v>1348.4</v>
       </c>
-      <c r="I113" s="10">
+      <c r="I113" s="8">
         <f>STDEV(H114:H123)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="J113" s="10">
+      <c r="J113" s="8">
         <f>MAX(H114:H123)-MIN(H114:H123)</f>
         <v>2</v>
       </c>
@@ -5934,11 +6443,11 @@
         <f>AVERAGE(M114:M123)</f>
         <v>2533</v>
       </c>
-      <c r="O113" s="10">
+      <c r="O113" s="8">
         <f>STDEV(N114:N123)</f>
         <v>1.699673171197595</v>
       </c>
-      <c r="P113" s="10">
+      <c r="P113" s="8">
         <f>MAX(N114:N123)-MIN(N114:N123)</f>
         <v>6</v>
       </c>
@@ -5953,11 +6462,11 @@
         <f>AVERAGE(S114:S123)</f>
         <v>2220.6</v>
       </c>
-      <c r="U113" s="10">
+      <c r="U113" s="8">
         <f>STDEV(T114:T123)</f>
         <v>1.5634719199411433</v>
       </c>
-      <c r="V113" s="10">
+      <c r="V113" s="8">
         <f>MAX(T114:T123)-MIN(T114:T123)</f>
         <v>6</v>
       </c>
@@ -6324,11 +6833,11 @@
         <f>AVERAGE(A125:A134)</f>
         <v>1776.4</v>
       </c>
-      <c r="C124" s="10">
+      <c r="C124" s="8">
         <f>STDEV(B125:B134)</f>
         <v>1.8287822299126939</v>
       </c>
-      <c r="D124" s="10">
+      <c r="D124" s="8">
         <f>MAX(B125:B134)-MIN(B125:B134)</f>
         <v>5</v>
       </c>
@@ -6343,11 +6852,11 @@
         <f>AVERAGE(G125:G134)</f>
         <v>1290.0999999999999</v>
       </c>
-      <c r="I124" s="10">
+      <c r="I124" s="8">
         <f>STDEV(H125:H134)</f>
         <v>1.9465068427541912</v>
       </c>
-      <c r="J124" s="10">
+      <c r="J124" s="8">
         <f>MAX(H125:H134)-MIN(H125:H134)</f>
         <v>7</v>
       </c>
@@ -6362,11 +6871,11 @@
         <f>AVERAGE(M125:M134)</f>
         <v>2381.6</v>
       </c>
-      <c r="O124" s="10">
+      <c r="O124" s="8">
         <f>STDEV(N125:N134)</f>
         <v>1.1352924243950935</v>
       </c>
-      <c r="P124" s="10">
+      <c r="P124" s="8">
         <f>MAX(N125:N134)-MIN(N125:N134)</f>
         <v>4</v>
       </c>
@@ -6381,11 +6890,11 @@
         <f>AVERAGE(S125:S134)</f>
         <v>2100.3000000000002</v>
       </c>
-      <c r="U124" s="10">
+      <c r="U124" s="8">
         <f>STDEV(T125:T134)</f>
         <v>1.3374935098492589</v>
       </c>
-      <c r="V124" s="10">
+      <c r="V124" s="8">
         <f>MAX(T125:T134)-MIN(T125:T134)</f>
         <v>5</v>
       </c>
@@ -6752,11 +7261,11 @@
         <f>AVERAGE(A136:A145)</f>
         <v>1730.4</v>
       </c>
-      <c r="C135" s="10">
+      <c r="C135" s="8">
         <f>STDEV(B136:B145)</f>
         <v>0.70710678118654757</v>
       </c>
-      <c r="D135" s="10">
+      <c r="D135" s="8">
         <f>MAX(B136:B145)-MIN(B136:B145)</f>
         <v>2</v>
       </c>
@@ -6771,11 +7280,11 @@
         <f>AVERAGE(G136:G145)</f>
         <v>1239.7</v>
       </c>
-      <c r="I135" s="10">
+      <c r="I135" s="8">
         <f>STDEV(H136:H145)</f>
         <v>2.1628170930011112</v>
       </c>
-      <c r="J135" s="10">
+      <c r="J135" s="8">
         <f>MAX(H136:H145)-MIN(H136:H145)</f>
         <v>7</v>
       </c>
@@ -6790,11 +7299,11 @@
         <f>AVERAGE(M136:M145)</f>
         <v>2262.3000000000002</v>
       </c>
-      <c r="O135" s="10">
+      <c r="O135" s="8">
         <f>STDEV(N136:N145)</f>
         <v>0.82327260234856459</v>
       </c>
-      <c r="P135" s="10">
+      <c r="P135" s="8">
         <f>MAX(N136:N145)-MIN(N136:N145)</f>
         <v>3</v>
       </c>
@@ -6809,11 +7318,11 @@
         <f>AVERAGE(S136:S145)</f>
         <v>2003.8</v>
       </c>
-      <c r="U135" s="10">
+      <c r="U135" s="8">
         <f>STDEV(T136:T145)</f>
         <v>0.73786478737262196</v>
       </c>
-      <c r="V135" s="10">
+      <c r="V135" s="8">
         <f>MAX(T136:T145)-MIN(T136:T145)</f>
         <v>2</v>
       </c>
@@ -7180,11 +7689,11 @@
         <f>AVERAGE(A147:A156)</f>
         <v>1697</v>
       </c>
-      <c r="C146" s="10">
+      <c r="C146" s="8">
         <f>STDEV(B147:B156)</f>
         <v>1.2649110640673518</v>
       </c>
-      <c r="D146" s="10">
+      <c r="D146" s="8">
         <f>MAX(B147:B156)-MIN(B147:B156)</f>
         <v>5</v>
       </c>
@@ -7199,11 +7708,11 @@
         <f>AVERAGE(G147:G156)</f>
         <v>1200.5</v>
       </c>
-      <c r="I146" s="10">
+      <c r="I146" s="8">
         <f>STDEV(H147:H156)</f>
         <v>0.91893658347268148</v>
       </c>
-      <c r="J146" s="10">
+      <c r="J146" s="8">
         <f>MAX(H147:H156)-MIN(H147:H156)</f>
         <v>3</v>
       </c>
@@ -7218,11 +7727,11 @@
         <f>AVERAGE(M147:M156)</f>
         <v>2166.9</v>
       </c>
-      <c r="O146" s="10">
+      <c r="O146" s="8">
         <f>STDEV(N147:N156)</f>
         <v>1.3498971154211057</v>
       </c>
-      <c r="P146" s="10">
+      <c r="P146" s="8">
         <f>MAX(N147:N156)-MIN(N147:N156)</f>
         <v>5</v>
       </c>
@@ -7237,11 +7746,11 @@
         <f>AVERAGE(S147:S156)</f>
         <v>1927.1</v>
       </c>
-      <c r="U146" s="10">
+      <c r="U146" s="8">
         <f>STDEV(T147:T156)</f>
         <v>0.84327404271156792</v>
       </c>
-      <c r="V146" s="10">
+      <c r="V146" s="8">
         <f>MAX(T147:T156)-MIN(T147:T156)</f>
         <v>2</v>
       </c>
@@ -7608,11 +8117,11 @@
         <f>AVERAGE(A158:A167)</f>
         <v>1669.5</v>
       </c>
-      <c r="C157" s="10">
+      <c r="C157" s="8">
         <f>STDEV(B158:B167)</f>
         <v>1.2866839377079189</v>
       </c>
-      <c r="D157" s="10">
+      <c r="D157" s="8">
         <f>MAX(B158:B167)-MIN(B158:B167)</f>
         <v>4</v>
       </c>
@@ -7627,11 +8136,11 @@
         <f>AVERAGE(G158:G167)</f>
         <v>1167.9000000000001</v>
       </c>
-      <c r="I157" s="10">
+      <c r="I157" s="8">
         <f>STDEV(H158:H167)</f>
         <v>1.6193277068654828</v>
       </c>
-      <c r="J157" s="10">
+      <c r="J157" s="8">
         <f>MAX(H158:H167)-MIN(H158:H167)</f>
         <v>6</v>
       </c>
@@ -7646,11 +8155,11 @@
         <f>AVERAGE(M158:M167)</f>
         <v>2089.4</v>
       </c>
-      <c r="O157" s="10">
+      <c r="O157" s="8">
         <f>STDEV(N158:N167)</f>
         <v>1.2649110640673518</v>
       </c>
-      <c r="P157" s="10">
+      <c r="P157" s="8">
         <f>MAX(N158:N167)-MIN(N158:N167)</f>
         <v>4</v>
       </c>
@@ -7665,11 +8174,11 @@
         <f>AVERAGE(S158:S167)</f>
         <v>1867.9</v>
       </c>
-      <c r="U157" s="10">
+      <c r="U157" s="8">
         <f>STDEV(T158:T167)</f>
         <v>0.63245553203367588</v>
       </c>
-      <c r="V157" s="10">
+      <c r="V157" s="8">
         <f>MAX(T158:T167)-MIN(T158:T167)</f>
         <v>2</v>
       </c>
@@ -8036,11 +8545,11 @@
         <f>AVERAGE(A169:A178)</f>
         <v>1642.2</v>
       </c>
-      <c r="C168" s="10">
+      <c r="C168" s="8">
         <f>STDEV(B169:B178)</f>
         <v>0.78881063774661553</v>
       </c>
-      <c r="D168" s="10">
+      <c r="D168" s="8">
         <f>MAX(B169:B178)-MIN(B169:B178)</f>
         <v>2</v>
       </c>
@@ -8055,11 +8564,11 @@
         <f>AVERAGE(G169:G178)</f>
         <v>1137.0999999999999</v>
       </c>
-      <c r="I168" s="10">
+      <c r="I168" s="8">
         <f>STDEV(H169:H178)</f>
         <v>1.1972189997378648</v>
       </c>
-      <c r="J168" s="10">
+      <c r="J168" s="8">
         <f>MAX(H169:H178)-MIN(H169:H178)</f>
         <v>3</v>
       </c>
@@ -8074,11 +8583,11 @@
         <f>AVERAGE(M169:M178)</f>
         <v>2023.4</v>
       </c>
-      <c r="O168" s="10">
+      <c r="O168" s="8">
         <f>STDEV(N169:N178)</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="P168" s="10">
+      <c r="P168" s="8">
         <f>MAX(N169:N178)-MIN(N169:N178)</f>
         <v>5</v>
       </c>
@@ -8093,11 +8602,11 @@
         <f>AVERAGE(S169:S178)</f>
         <v>1811.5</v>
       </c>
-      <c r="U168" s="10">
+      <c r="U168" s="8">
         <f>STDEV(T169:T178)</f>
         <v>1.3984117975602022</v>
       </c>
-      <c r="V168" s="10">
+      <c r="V168" s="8">
         <f>MAX(T169:T178)-MIN(T169:T178)</f>
         <v>5</v>
       </c>
@@ -8464,11 +8973,11 @@
         <f>AVERAGE(A180:A189)</f>
         <v>1622.5</v>
       </c>
-      <c r="C179" s="10">
+      <c r="C179" s="8">
         <f>STDEV(B180:B189)</f>
         <v>1.2649110640673518</v>
       </c>
-      <c r="D179" s="10">
+      <c r="D179" s="8">
         <f>MAX(B180:B189)-MIN(B180:B189)</f>
         <v>4</v>
       </c>
@@ -8483,11 +8992,11 @@
         <f>AVERAGE(G180:G189)</f>
         <v>1114.2</v>
       </c>
-      <c r="I179" s="10">
+      <c r="I179" s="8">
         <f>STDEV(H180:H189)</f>
         <v>1.4491376746189439</v>
       </c>
-      <c r="J179" s="10">
+      <c r="J179" s="8">
         <f>MAX(H180:H189)-MIN(H180:H189)</f>
         <v>5</v>
       </c>
@@ -8502,11 +9011,11 @@
         <f>AVERAGE(M180:M189)</f>
         <v>1974.5</v>
       </c>
-      <c r="O179" s="10">
+      <c r="O179" s="8">
         <f>STDEV(N180:N189)</f>
         <v>0.94280904158206336</v>
       </c>
-      <c r="P179" s="10">
+      <c r="P179" s="8">
         <f>MAX(N180:N189)-MIN(N180:N189)</f>
         <v>3</v>
       </c>
@@ -8521,11 +9030,11 @@
         <f>AVERAGE(S180:S189)</f>
         <v>1771.2</v>
       </c>
-      <c r="U179" s="10">
+      <c r="U179" s="8">
         <f>STDEV(T180:T189)</f>
         <v>1.1547005383792515</v>
       </c>
-      <c r="V179" s="10">
+      <c r="V179" s="8">
         <f>MAX(T180:T189)-MIN(T180:T189)</f>
         <v>4</v>
       </c>
@@ -8892,11 +9401,11 @@
         <f>AVERAGE(A191:A200)</f>
         <v>1606</v>
       </c>
-      <c r="C190" s="10">
+      <c r="C190" s="8">
         <f>STDEV(B191:B200)</f>
         <v>0.73786478737262196</v>
       </c>
-      <c r="D190" s="10">
+      <c r="D190" s="8">
         <f>MAX(B191:B200)-MIN(B191:B200)</f>
         <v>3</v>
       </c>
@@ -8911,11 +9420,11 @@
         <f>AVERAGE(G191:G200)</f>
         <v>1094.2</v>
       </c>
-      <c r="I190" s="10">
+      <c r="I190" s="8">
         <f>STDEV(H191:H200)</f>
         <v>1.2292725943057186</v>
       </c>
-      <c r="J190" s="10">
+      <c r="J190" s="8">
         <f>MAX(H191:H200)-MIN(H191:H200)</f>
         <v>4</v>
       </c>
@@ -8930,11 +9439,11 @@
         <f>AVERAGE(M191:M200)</f>
         <v>1929.5</v>
       </c>
-      <c r="O190" s="10">
+      <c r="O190" s="8">
         <f>STDEV(N191:N200)</f>
         <v>1.5951314818673865</v>
       </c>
-      <c r="P190" s="10">
+      <c r="P190" s="8">
         <f>MAX(N191:N200)-MIN(N191:N200)</f>
         <v>5</v>
       </c>
@@ -8949,11 +9458,11 @@
         <f>AVERAGE(S191:S200)</f>
         <v>1739</v>
       </c>
-      <c r="U190" s="10">
+      <c r="U190" s="8">
         <f>STDEV(T191:T200)</f>
         <v>1.7669811040931429</v>
       </c>
-      <c r="V190" s="10">
+      <c r="V190" s="8">
         <f>MAX(T191:T200)-MIN(T191:T200)</f>
         <v>6</v>
       </c>
@@ -9320,11 +9829,11 @@
         <f>AVERAGE(A202:A211)</f>
         <v>1590.6</v>
       </c>
-      <c r="C201" s="10">
+      <c r="C201" s="8">
         <f>STDEV(B202:B211)</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="D201" s="10">
+      <c r="D201" s="8">
         <f>MAX(B202:B211)-MIN(B202:B211)</f>
         <v>4</v>
       </c>
@@ -9339,11 +9848,11 @@
         <f>AVERAGE(G202:G211)</f>
         <v>1076.0999999999999</v>
       </c>
-      <c r="I201" s="10">
+      <c r="I201" s="8">
         <f>STDEV(H202:H211)</f>
         <v>1.5811388300841898</v>
       </c>
-      <c r="J201" s="10">
+      <c r="J201" s="8">
         <f>MAX(H202:H211)-MIN(H202:H211)</f>
         <v>5</v>
       </c>
@@ -9358,11 +9867,11 @@
         <f>AVERAGE(M202:M211)</f>
         <v>1890.5</v>
       </c>
-      <c r="O201" s="10">
+      <c r="O201" s="8">
         <f>STDEV(N202:N211)</f>
         <v>1.2516655570345725</v>
       </c>
-      <c r="P201" s="10">
+      <c r="P201" s="8">
         <f>MAX(N202:N211)-MIN(N202:N211)</f>
         <v>4</v>
       </c>
@@ -9377,11 +9886,11 @@
         <f>AVERAGE(S202:S211)</f>
         <v>1709.9</v>
       </c>
-      <c r="U201" s="10">
+      <c r="U201" s="8">
         <f>STDEV(T202:T211)</f>
         <v>1.1737877907772674</v>
       </c>
-      <c r="V201" s="10">
+      <c r="V201" s="8">
         <f>MAX(T202:T211)-MIN(T202:T211)</f>
         <v>4</v>
       </c>
@@ -9748,11 +10257,11 @@
         <f>AVERAGE(A213:A222)</f>
         <v>1578.2</v>
       </c>
-      <c r="C212" s="10">
+      <c r="C212" s="8">
         <f>STDEV(B213:B222)</f>
         <v>0.94280904158206336</v>
       </c>
-      <c r="D212" s="10">
+      <c r="D212" s="8">
         <f>MAX(B213:B222)-MIN(B213:B222)</f>
         <v>3</v>
       </c>
@@ -9767,11 +10276,11 @@
         <f>AVERAGE(G213:G222)</f>
         <v>1061.7</v>
       </c>
-      <c r="I212" s="10">
+      <c r="I212" s="8">
         <f>STDEV(H213:H222)</f>
         <v>1.1595018087284057</v>
       </c>
-      <c r="J212" s="10">
+      <c r="J212" s="8">
         <f>MAX(H213:H222)-MIN(H213:H222)</f>
         <v>4</v>
       </c>
@@ -9786,11 +10295,11 @@
         <f>AVERAGE(M213:M222)</f>
         <v>1861.9</v>
       </c>
-      <c r="O212" s="10">
+      <c r="O212" s="8">
         <f>STDEV(N213:N222)</f>
         <v>0.31622776601683794</v>
       </c>
-      <c r="P212" s="10">
+      <c r="P212" s="8">
         <f>MAX(N213:N222)-MIN(N213:N222)</f>
         <v>1</v>
       </c>
@@ -9805,11 +10314,11 @@
         <f>AVERAGE(S213:S222)</f>
         <v>1686.6</v>
       </c>
-      <c r="U212" s="10">
+      <c r="U212" s="8">
         <f>STDEV(T213:T222)</f>
         <v>2</v>
       </c>
-      <c r="V212" s="10">
+      <c r="V212" s="8">
         <f>MAX(T213:T222)-MIN(T213:T222)</f>
         <v>8</v>
       </c>
@@ -10176,11 +10685,11 @@
         <f>AVERAGE(A224:A233)</f>
         <v>1568</v>
       </c>
-      <c r="C223" s="10">
+      <c r="C223" s="8">
         <f>STDEV(B224:B233)</f>
         <v>1.2292725943057186</v>
       </c>
-      <c r="D223" s="10">
+      <c r="D223" s="8">
         <f>MAX(B224:B233)-MIN(B224:B233)</f>
         <v>4</v>
       </c>
@@ -10195,11 +10704,11 @@
         <f>AVERAGE(G224:G233)</f>
         <v>1048.9000000000001</v>
       </c>
-      <c r="I223" s="10">
+      <c r="I223" s="8">
         <f>STDEV(H224:H233)</f>
         <v>1.1785113019775793</v>
       </c>
-      <c r="J223" s="10">
+      <c r="J223" s="8">
         <f>MAX(H224:H233)-MIN(H224:H233)</f>
         <v>3</v>
       </c>
@@ -10214,11 +10723,11 @@
         <f>AVERAGE(M224:M233)</f>
         <v>1832.7</v>
       </c>
-      <c r="O223" s="10">
+      <c r="O223" s="8">
         <f>STDEV(N224:N233)</f>
         <v>1.1972189997378648</v>
       </c>
-      <c r="P223" s="10">
+      <c r="P223" s="8">
         <f>MAX(N224:N233)-MIN(N224:N233)</f>
         <v>4</v>
       </c>
@@ -10233,11 +10742,11 @@
         <f>AVERAGE(S224:S233)</f>
         <v>1666.2</v>
       </c>
-      <c r="U223" s="10">
+      <c r="U223" s="8">
         <f>STDEV(T224:T233)</f>
         <v>1.3374935098492589</v>
       </c>
-      <c r="V223" s="10">
+      <c r="V223" s="8">
         <f>MAX(T224:T233)-MIN(T224:T233)</f>
         <v>5</v>
       </c>
@@ -10604,11 +11113,11 @@
         <f>AVERAGE(A235:A244)</f>
         <v>1559.8</v>
       </c>
-      <c r="C234" s="10">
+      <c r="C234" s="8">
         <f>STDEV(B235:B244)</f>
         <v>1.4142135623730951</v>
       </c>
-      <c r="D234" s="10">
+      <c r="D234" s="8">
         <f>MAX(B235:B244)-MIN(B235:B244)</f>
         <v>4</v>
       </c>
@@ -10623,11 +11132,11 @@
         <f>AVERAGE(G235:G244)</f>
         <v>1039.5999999999999</v>
       </c>
-      <c r="I234" s="10">
+      <c r="I234" s="8">
         <f>STDEV(H235:H244)</f>
         <v>0.97182531580755005</v>
       </c>
-      <c r="J234" s="10">
+      <c r="J234" s="8">
         <f>MAX(H235:H244)-MIN(H235:H244)</f>
         <v>3</v>
       </c>
@@ -10642,11 +11151,11 @@
         <f>AVERAGE(M235:M244)</f>
         <v>1808.7</v>
       </c>
-      <c r="O234" s="10">
+      <c r="O234" s="8">
         <f>STDEV(N235:N244)</f>
         <v>0.48304589153964794</v>
       </c>
-      <c r="P234" s="10">
+      <c r="P234" s="8">
         <f>MAX(N235:N244)-MIN(N235:N244)</f>
         <v>1</v>
       </c>
@@ -10661,11 +11170,11 @@
         <f>AVERAGE(S235:S244)</f>
         <v>1648.5</v>
       </c>
-      <c r="U234" s="10">
+      <c r="U234" s="8">
         <f>STDEV(T235:T244)</f>
         <v>0.67494855771055284</v>
       </c>
-      <c r="V234" s="10">
+      <c r="V234" s="8">
         <f>MAX(T235:T244)-MIN(T235:T244)</f>
         <v>2</v>
       </c>
@@ -11032,11 +11541,11 @@
         <f>AVERAGE(A246:A255)</f>
         <v>1552.2</v>
       </c>
-      <c r="C245" s="10">
+      <c r="C245" s="8">
         <f>STDEV(B246:B255)</f>
         <v>1.4491376746189437</v>
       </c>
-      <c r="D245" s="10">
+      <c r="D245" s="8">
         <f>MAX(B246:B255)-MIN(B246:B255)</f>
         <v>5</v>
       </c>
@@ -11051,11 +11560,11 @@
         <f>AVERAGE(G246:G255)</f>
         <v>1029.2</v>
       </c>
-      <c r="I245" s="10">
+      <c r="I245" s="8">
         <f>STDEV(H246:H255)</f>
         <v>0.82327260234856459</v>
       </c>
-      <c r="J245" s="10">
+      <c r="J245" s="8">
         <f>MAX(H246:H255)-MIN(H246:H255)</f>
         <v>3</v>
       </c>
@@ -11070,11 +11579,11 @@
         <f>AVERAGE(M246:M255)</f>
         <v>1791.8</v>
       </c>
-      <c r="O245" s="10">
+      <c r="O245" s="8">
         <f>STDEV(N246:N255)</f>
         <v>1.2866839377079189</v>
       </c>
-      <c r="P245" s="10">
+      <c r="P245" s="8">
         <f>MAX(N246:N255)-MIN(N246:N255)</f>
         <v>5</v>
       </c>
@@ -11089,11 +11598,11 @@
         <f>AVERAGE(S246:S255)</f>
         <v>1635.2</v>
       </c>
-      <c r="U245" s="10">
+      <c r="U245" s="8">
         <f>STDEV(T246:T255)</f>
         <v>0.42163702135578385</v>
       </c>
-      <c r="V245" s="10">
+      <c r="V245" s="8">
         <f>MAX(T246:T255)-MIN(T246:T255)</f>
         <v>1</v>
       </c>
@@ -11460,11 +11969,11 @@
         <f>AVERAGE(A257:A266)</f>
         <v>1544.6</v>
       </c>
-      <c r="C256" s="10">
+      <c r="C256" s="8">
         <f>STDEV(B257:B266)</f>
         <v>0.94280904158206336</v>
       </c>
-      <c r="D256" s="10">
+      <c r="D256" s="8">
         <f>MAX(B257:B266)-MIN(B257:B266)</f>
         <v>3</v>
       </c>
@@ -11479,11 +11988,11 @@
         <f>AVERAGE(G257:G266)</f>
         <v>1019.4</v>
       </c>
-      <c r="I256" s="10">
+      <c r="I256" s="8">
         <f>STDEV(H257:H266)</f>
         <v>1.1005049346146119</v>
       </c>
-      <c r="J256" s="10">
+      <c r="J256" s="8">
         <f>MAX(H257:H266)-MIN(H257:H266)</f>
         <v>3</v>
       </c>
@@ -11498,11 +12007,11 @@
         <f>AVERAGE(M257:M266)</f>
         <v>1771.4</v>
       </c>
-      <c r="O256" s="10">
+      <c r="O256" s="8">
         <f>STDEV(N257:N266)</f>
         <v>0.94868329805051388</v>
       </c>
-      <c r="P256" s="10">
+      <c r="P256" s="8">
         <f>MAX(N257:N266)-MIN(N257:N266)</f>
         <v>3</v>
       </c>
@@ -11517,11 +12026,11 @@
         <f>AVERAGE(S257:S266)</f>
         <v>1621.4</v>
       </c>
-      <c r="U256" s="10">
+      <c r="U256" s="8">
         <f>STDEV(T257:T266)</f>
         <v>0.73786478737262196</v>
       </c>
-      <c r="V256" s="10">
+      <c r="V256" s="8">
         <f>MAX(T257:T266)-MIN(T257:T266)</f>
         <v>2</v>
       </c>
@@ -11888,11 +12397,11 @@
         <f>AVERAGE(A268:A277)</f>
         <v>1537.7</v>
       </c>
-      <c r="C267" s="10">
+      <c r="C267" s="8">
         <f>STDEV(B268:B277)</f>
         <v>0.91893658347268148</v>
       </c>
-      <c r="D267" s="10">
+      <c r="D267" s="8">
         <f>MAX(B268:B277)-MIN(B268:B277)</f>
         <v>3</v>
       </c>
@@ -11907,11 +12416,11 @@
         <f>AVERAGE(G268:G277)</f>
         <v>1012.4</v>
       </c>
-      <c r="I267" s="10">
+      <c r="I267" s="8">
         <f>STDEV(H268:H277)</f>
         <v>0.91893658347268148</v>
       </c>
-      <c r="J267" s="10">
+      <c r="J267" s="8">
         <f>MAX(H268:H277)-MIN(H268:H277)</f>
         <v>3</v>
       </c>
@@ -11926,11 +12435,11 @@
         <f>AVERAGE(M268:M277)</f>
         <v>1755.5</v>
       </c>
-      <c r="O267" s="10">
+      <c r="O267" s="8">
         <f>STDEV(N268:N277)</f>
         <v>1.5811388300841898</v>
       </c>
-      <c r="P267" s="10">
+      <c r="P267" s="8">
         <f>MAX(N268:N277)-MIN(N268:N277)</f>
         <v>5</v>
       </c>
@@ -11945,11 +12454,11 @@
         <f>AVERAGE(S268:S277)</f>
         <v>1610.4</v>
       </c>
-      <c r="U267" s="10">
+      <c r="U267" s="8">
         <f>STDEV(T268:T277)</f>
         <v>0.67494855771055284</v>
       </c>
-      <c r="V267" s="10">
+      <c r="V267" s="8">
         <f>MAX(T268:T277)-MIN(T268:T277)</f>
         <v>2</v>
       </c>
@@ -12316,11 +12825,11 @@
         <f>AVERAGE(A279:A288)</f>
         <v>1532.6</v>
       </c>
-      <c r="C278" s="10">
+      <c r="C278" s="8">
         <f>STDEV(B279:B288)</f>
         <v>0.73786478737262196</v>
       </c>
-      <c r="D278" s="10">
+      <c r="D278" s="8">
         <f>MAX(B279:B288)-MIN(B279:B288)</f>
         <v>2</v>
       </c>
@@ -12335,11 +12844,11 @@
         <f>AVERAGE(G279:G288)</f>
         <v>1005.7</v>
       </c>
-      <c r="I278" s="10">
+      <c r="I278" s="8">
         <f>STDEV(H279:H288)</f>
         <v>0.84327404271156792</v>
       </c>
-      <c r="J278" s="10">
+      <c r="J278" s="8">
         <f>MAX(H279:H288)-MIN(H279:H288)</f>
         <v>3</v>
       </c>
@@ -12354,11 +12863,11 @@
         <f>AVERAGE(M279:M288)</f>
         <v>1741.5</v>
       </c>
-      <c r="O278" s="10">
+      <c r="O278" s="8">
         <f>STDEV(N279:N288)</f>
         <v>0.94868329805051377</v>
       </c>
-      <c r="P278" s="10">
+      <c r="P278" s="8">
         <f>MAX(N279:N288)-MIN(N279:N288)</f>
         <v>3</v>
       </c>
@@ -12373,11 +12882,11 @@
         <f>AVERAGE(S279:S288)</f>
         <v>1600.6</v>
       </c>
-      <c r="U278" s="10">
+      <c r="U278" s="8">
         <f>STDEV(T279:T288)</f>
         <v>1.0593499054713802</v>
       </c>
-      <c r="V278" s="10">
+      <c r="V278" s="8">
         <f>MAX(T279:T288)-MIN(T279:T288)</f>
         <v>3</v>
       </c>
@@ -12744,11 +13253,11 @@
         <f>AVERAGE(A290:A299)</f>
         <v>1528.2</v>
       </c>
-      <c r="C289" s="10">
+      <c r="C289" s="8">
         <f>STDEV(B290:B299)</f>
         <v>1.1005049346146119</v>
       </c>
-      <c r="D289" s="10">
+      <c r="D289" s="8">
         <f>MAX(B290:B299)-MIN(B290:B299)</f>
         <v>4</v>
       </c>
@@ -12763,11 +13272,11 @@
         <f>AVERAGE(G290:G299)</f>
         <v>1000.1</v>
       </c>
-      <c r="I289" s="10">
+      <c r="I289" s="8">
         <f>STDEV(H290:H299)</f>
         <v>1.3703203194062976</v>
       </c>
-      <c r="J289" s="10">
+      <c r="J289" s="8">
         <f>MAX(H290:H299)-MIN(H290:H299)</f>
         <v>5</v>
       </c>
@@ -12782,11 +13291,11 @@
         <f>AVERAGE(M290:M299)</f>
         <v>1729.6</v>
       </c>
-      <c r="O289" s="10">
+      <c r="O289" s="8">
         <f>STDEV(N290:N299)</f>
         <v>0.99442892601175337</v>
       </c>
-      <c r="P289" s="10">
+      <c r="P289" s="8">
         <f>MAX(N290:N299)-MIN(N290:N299)</f>
         <v>3</v>
       </c>
@@ -12801,11 +13310,11 @@
         <f>AVERAGE(S290:S299)</f>
         <v>1590.6</v>
       </c>
-      <c r="U289" s="10">
+      <c r="U289" s="8">
         <f>STDEV(T290:T299)</f>
         <v>0.67494855771055284</v>
       </c>
-      <c r="V289" s="10">
+      <c r="V289" s="8">
         <f>MAX(T290:T299)-MIN(T290:T299)</f>
         <v>2</v>
       </c>
@@ -13172,11 +13681,11 @@
         <f>AVERAGE(A301:A310)</f>
         <v>1524.9</v>
       </c>
-      <c r="C300" s="10">
+      <c r="C300" s="8">
         <f>STDEV(B301:B310)</f>
         <v>0.4216370213557839</v>
       </c>
-      <c r="D300" s="10">
+      <c r="D300" s="8">
         <f>MAX(B301:B310)-MIN(B301:B310)</f>
         <v>1</v>
       </c>
@@ -13191,11 +13700,11 @@
         <f>AVERAGE(G301:G310)</f>
         <v>995.2</v>
       </c>
-      <c r="I300" s="10">
+      <c r="I300" s="8">
         <f>STDEV(H301:H310)</f>
         <v>0.73786478737262184</v>
       </c>
-      <c r="J300" s="10">
+      <c r="J300" s="8">
         <f>MAX(H301:H310)-MIN(H301:H310)</f>
         <v>3</v>
       </c>
@@ -13210,11 +13719,11 @@
         <f>AVERAGE(M301:M310)</f>
         <v>1719.1</v>
       </c>
-      <c r="O300" s="10">
+      <c r="O300" s="8">
         <f>STDEV(N301:N310)</f>
         <v>1.2692955176439846</v>
       </c>
-      <c r="P300" s="10">
+      <c r="P300" s="8">
         <f>MAX(N301:N310)-MIN(N301:N310)</f>
         <v>5</v>
       </c>
@@ -13229,11 +13738,11 @@
         <f>AVERAGE(S301:S310)</f>
         <v>1584.8</v>
       </c>
-      <c r="U300" s="10">
+      <c r="U300" s="8">
         <f>STDEV(T301:T310)</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="V300" s="10">
+      <c r="V300" s="8">
         <f>MAX(T301:T310)-MIN(T301:T310)</f>
         <v>5</v>
       </c>
@@ -13600,11 +14109,11 @@
         <f>AVERAGE(A312:A321)</f>
         <v>1520.8</v>
       </c>
-      <c r="C311" s="10">
+      <c r="C311" s="8">
         <f>STDEV(B312:B321)</f>
         <v>0.31622776601683794</v>
       </c>
-      <c r="D311" s="10">
+      <c r="D311" s="8">
         <f>MAX(B312:B321)-MIN(B312:B321)</f>
         <v>1</v>
       </c>
@@ -13619,11 +14128,11 @@
         <f>AVERAGE(G312:G321)</f>
         <v>992.3</v>
       </c>
-      <c r="I311" s="10">
+      <c r="I311" s="8">
         <f>STDEV(H312:H321)</f>
         <v>0.966091783079296</v>
       </c>
-      <c r="J311" s="10">
+      <c r="J311" s="8">
         <f>MAX(H312:H321)-MIN(H312:H321)</f>
         <v>3</v>
       </c>
@@ -13638,11 +14147,11 @@
         <f>AVERAGE(M312:M321)</f>
         <v>1709.6</v>
       </c>
-      <c r="O311" s="10">
+      <c r="O311" s="8">
         <f>STDEV(N312:N321)</f>
         <v>1.4142135623730951</v>
       </c>
-      <c r="P311" s="10">
+      <c r="P311" s="8">
         <f>MAX(N312:N321)-MIN(N312:N321)</f>
         <v>5</v>
       </c>
@@ -13657,11 +14166,11 @@
         <f>AVERAGE(S312:S321)</f>
         <v>1576</v>
       </c>
-      <c r="U311" s="10">
+      <c r="U311" s="8">
         <f>STDEV(T312:T321)</f>
         <v>1.7288403306519917</v>
       </c>
-      <c r="V311" s="10">
+      <c r="V311" s="8">
         <f>MAX(T312:T321)-MIN(T312:T321)</f>
         <v>6</v>
       </c>
@@ -14028,11 +14537,11 @@
         <f>AVERAGE(A323:A332)</f>
         <v>1519.1</v>
       </c>
-      <c r="C322" s="10">
+      <c r="C322" s="8">
         <f>STDEV(B323:B332)</f>
         <v>1.247219128924647</v>
       </c>
-      <c r="D322" s="10">
+      <c r="D322" s="8">
         <f>MAX(B323:B332)-MIN(B323:B332)</f>
         <v>4</v>
       </c>
@@ -14047,11 +14556,11 @@
         <f>AVERAGE(G323:G332)</f>
         <v>987.6</v>
       </c>
-      <c r="I322" s="10">
+      <c r="I322" s="8">
         <f>STDEV(H323:H332)</f>
         <v>1.3165611772087669</v>
       </c>
-      <c r="J322" s="10">
+      <c r="J322" s="8">
         <f>MAX(H323:H332)-MIN(H323:H332)</f>
         <v>5</v>
       </c>
@@ -14066,11 +14575,11 @@
         <f>AVERAGE(M323:M332)</f>
         <v>1701.8</v>
       </c>
-      <c r="O322" s="10">
+      <c r="O322" s="8">
         <f>STDEV(N323:N332)</f>
         <v>0.56764621219754674</v>
       </c>
-      <c r="P322" s="10">
+      <c r="P322" s="8">
         <f>MAX(N323:N332)-MIN(N323:N332)</f>
         <v>2</v>
       </c>
@@ -14085,11 +14594,11 @@
         <f>AVERAGE(S323:S332)</f>
         <v>1570.2</v>
       </c>
-      <c r="U322" s="10">
+      <c r="U322" s="8">
         <f>STDEV(T323:T332)</f>
         <v>0.81649658092772603</v>
       </c>
-      <c r="V322" s="10">
+      <c r="V322" s="8">
         <f>MAX(T323:T332)-MIN(T323:T332)</f>
         <v>2</v>
       </c>
@@ -14426,7 +14935,7 @@
     <mergeCell ref="G1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -14439,7 +14948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>

</xml_diff>

<commit_message>
generated linear eq for sensors
</commit_message>
<xml_diff>
--- a/experiments/SensorGraph.xlsx
+++ b/experiments/SensorGraph.xlsx
@@ -4,11 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="4000" yWindow="2400" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sensor Readings" sheetId="1" r:id="rId1"/>
     <sheet name="Graph" sheetId="2" r:id="rId2"/>
+    <sheet name="Right Sensor" sheetId="4" r:id="rId3"/>
+    <sheet name="Left Sensor" sheetId="3" r:id="rId4"/>
+    <sheet name="Right Center Sensor" sheetId="5" r:id="rId5"/>
+    <sheet name="Left Center Sensor" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -94,12 +98,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,7 +148,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -160,6 +170,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -216,16 +231,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Right Sensor</c:v>
+          </c:tx>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="3"/>
+            <c:order val="6"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.103448275862069"/>
-                  <c:y val="-0.290476917129545"/>
+                  <c:x val="0.0797913618098623"/>
+                  <c:y val="0.018790097183798"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -233,10 +251,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$G$3:$G$58</c:f>
+              <c:f>'Sensor Readings'!$S$3:$S$322</c:f>
               <c:numCache>
                 <c:formatCode>0" cm"</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -254,33 +272,177 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$H$3:$H$58</c:f>
+              <c:f>'Sensor Readings'!$B$3:$B$322</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>3620.4</c:v>
+                  <c:v>3641.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3455.5</c:v>
+                  <c:v>3500.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3003.8</c:v>
+                  <c:v>3237.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2523.9</c:v>
+                  <c:v>2833.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2165.2</c:v>
+                  <c:v>2584.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1914.5</c:v>
+                  <c:v>2334.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2170.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2041.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1951.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1879.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1823.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1776.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1730.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1697.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1669.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1642.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1622.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1606.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1590.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1578.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1568.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1559.8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1552.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1544.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1537.7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1532.6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1528.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1524.9</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1520.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1519.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -290,16 +452,19 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Left Sensor</c:v>
+          </c:tx>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="6"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0706983946510996"/>
-                  <c:y val="-0.00921849885043439"/>
+                  <c:x val="0.0701631709753095"/>
+                  <c:y val="0.0309894303752571"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -307,54 +472,198 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$G$58:$G$113</c:f>
+              <c:f>'Sensor Readings'!$S$3:$S$322</c:f>
               <c:numCache>
                 <c:formatCode>0" cm"</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>6.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>7.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>8.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>9.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$H$58:$H$113</c:f>
+              <c:f>'Sensor Readings'!$H$3:$H$322</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>3620.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3455.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3003.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2523.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2165.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1914.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>1748.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>1612.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="8">
                   <c:v>1511.9</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="9">
                   <c:v>1412.4</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>1348.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1290.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1239.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1200.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1167.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1137.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1114.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1094.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1076.1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1061.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1048.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1039.6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1029.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1019.4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1012.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1005.7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1000.1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>995.2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>992.3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>987.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -364,16 +673,19 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Right Center Sensor</c:v>
+          </c:tx>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="5"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.0824202416508281"/>
-                  <c:y val="-0.0591993733341472"/>
+                  <c:x val="-0.249912549648108"/>
+                  <c:y val="-0.220794920905157"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -381,54 +693,198 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$G$113:$G$168</c:f>
+              <c:f>'Sensor Readings'!$S$3:$S$322</c:f>
               <c:numCache>
                 <c:formatCode>0" cm"</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>10.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>11.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
                   <c:v>12.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="13">
                   <c:v>13.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>14.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="15">
                   <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$H$113:$H$168</c:f>
+              <c:f>'Sensor Readings'!$N$3:$N$322</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>1348.4</c:v>
+                  <c:v>3823.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1290.1</c:v>
+                  <c:v>3885.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1239.7</c:v>
+                  <c:v>3860.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1200.5</c:v>
+                  <c:v>3818.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1167.9</c:v>
+                  <c:v>3771.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1137.1</c:v>
+                  <c:v>3660.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3515.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3285.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2995.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2718.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2533.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2381.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2262.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2166.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2089.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2023.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1974.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1929.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1890.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1861.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1832.7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1808.7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1791.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1771.4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1755.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1741.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1729.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1719.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1709.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1701.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -438,16 +894,19 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:v>Left Center Sensor</c:v>
+          </c:tx>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="6"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0112175875644855"/>
-                  <c:y val="0.0317328938533846"/>
+                  <c:x val="0.118113197686572"/>
+                  <c:y val="-0.105774420089381"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -455,152 +914,198 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$G$168:$G$223</c:f>
+              <c:f>'Sensor Readings'!$S$3:$S$322</c:f>
               <c:numCache>
                 <c:formatCode>0" cm"</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>15.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="16">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="17">
                   <c:v>17.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="18">
                   <c:v>18.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="19">
                   <c:v>19.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="20">
                   <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$H$168:$H$223</c:f>
+              <c:f>'Sensor Readings'!$T$3:$T$322</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>1137.1</c:v>
+                  <c:v>3860.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1114.2</c:v>
+                  <c:v>3884.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1094.2</c:v>
+                  <c:v>3843.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1076.1</c:v>
+                  <c:v>3783.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1061.7</c:v>
+                  <c:v>3663.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1048.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:trendline>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.0180597508824328"/>
-                  <c:y val="-0.0620273047264441"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Sensor Readings'!$G$223:$G$322</c:f>
-              <c:numCache>
-                <c:formatCode>0" cm"</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25.0</c:v>
+                  <c:v>3492.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.0</c:v>
+                  <c:v>3212.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.0</c:v>
+                  <c:v>2840.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28.0</c:v>
+                  <c:v>2560.7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Sensor Readings'!$H$223:$H$322</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1048.9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1039.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1029.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1019.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1012.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1005.7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1000.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>995.2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>992.3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>987.6</c:v>
+                  <c:v>2367.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2220.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2100.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2003.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1927.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1867.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1811.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1771.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1739.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1709.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1686.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1666.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1648.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1635.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1621.4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1610.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1600.6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1590.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1584.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1576.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1570.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -615,11 +1120,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2074606808"/>
-        <c:axId val="2074617768"/>
+        <c:axId val="2061585624"/>
+        <c:axId val="2061582808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2074606808"/>
+        <c:axId val="2061585624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,12 +1134,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074617768"/>
+        <c:crossAx val="2061582808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2074617768"/>
+        <c:axId val="2061582808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -645,14 +1150,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074606808"/>
+        <c:crossAx val="2061585624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -691,18 +1195,18 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Right Sensor</c:v>
+            <c:v>0cm-5cm</c:v>
           </c:tx>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="6"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.0797913618098623"/>
-                  <c:y val="0.018790097183798"/>
+                  <c:x val="0.111353340139286"/>
+                  <c:y val="-0.0775026762138116"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -710,198 +1214,54 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$S$3:$S$322</c:f>
+              <c:f>'Sensor Readings'!$B$3:$B$58</c:f>
               <c:numCache>
-                <c:formatCode>0" cm"</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>3641.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>3500.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>3237.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>2833.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>2584.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29.0</c:v>
+                  <c:v>2334.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$B$3:$B$322</c:f>
+              <c:f>'Sensor Readings'!$A$3:$A$58</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3641.4</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3500.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3237.6</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2833.5</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2584.2</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2334.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2170.9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2041.6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1951.3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1879.6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1823.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1776.4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1730.4</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1697.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1669.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1642.2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1622.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1606.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1590.6</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1578.2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1568.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1559.8</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1552.2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1544.6</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1537.7</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1532.6</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1528.2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1524.9</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1520.8</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1519.1</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -912,18 +1272,18 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Left Sensor</c:v>
+            <c:v>5cm-10cm</c:v>
           </c:tx>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="6"/>
+            <c:order val="2"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.0701631709753095"/>
-                  <c:y val="0.0309894303752571"/>
+                  <c:x val="-0.0648562158228296"/>
+                  <c:y val="-0.0210769084378048"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -931,198 +1291,54 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$S$3:$S$322</c:f>
+              <c:f>'Sensor Readings'!$B$58:$B$113</c:f>
               <c:numCache>
-                <c:formatCode>0" cm"</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>2334.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>2170.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2041.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>1951.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>1879.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29.0</c:v>
+                  <c:v>1823.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$H$3:$H$322</c:f>
+              <c:f>'Sensor Readings'!$A$58:$A$113</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3620.4</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3455.5</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3003.8</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2523.9</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2165.2</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1914.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1748.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1612.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1511.9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1412.4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1348.4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1290.1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1239.7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1200.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1167.9</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1137.1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1114.2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1094.2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1076.1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1061.7</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1048.9</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1039.6</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1029.2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1019.4</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1012.4</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1005.7</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1000.1</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>995.2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>992.3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>987.6</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1133,217 +1349,68 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Right Center Sensor</c:v>
+            <c:v>10cm-15cm</c:v>
           </c:tx>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="5"/>
+            <c:order val="2"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.249912549648108"/>
-                  <c:y val="-0.220794920905157"/>
-                </c:manualLayout>
-              </c:layout>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$S$3:$S$322</c:f>
+              <c:f>'Sensor Readings'!$B$113:$B$168</c:f>
               <c:numCache>
-                <c:formatCode>0" cm"</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>1823.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1776.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>1730.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>1697.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>1669.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29.0</c:v>
+                  <c:v>1642.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$N$3:$N$322</c:f>
+              <c:f>'Sensor Readings'!$A$113:$A$168</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3823.2</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3885.2</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3860.8</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3818.2</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3771.7</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3660.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3515.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3285.2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2995.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2718.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2533.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2381.6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2262.3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2166.9</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2089.4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2023.4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1974.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1929.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1890.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1861.9</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1832.7</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1808.7</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1791.8</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1771.4</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1755.5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1741.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1729.6</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1719.1</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1709.6</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1701.8</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1354,217 +1421,208 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Left Center Sensor</c:v>
+            <c:v>15cm-20cm</c:v>
           </c:tx>
           <c:trendline>
-            <c:trendlineType val="poly"/>
-            <c:order val="6"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.118113197686572"/>
-                  <c:y val="-0.105774420089381"/>
-                </c:manualLayout>
-              </c:layout>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$S$3:$S$322</c:f>
+              <c:f>'Sensor Readings'!$B$168:$B$223</c:f>
               <c:numCache>
-                <c:formatCode>0" cm"</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>1642.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1622.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>1606.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>1590.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>1578.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>28.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>29.0</c:v>
+                  <c:v>1568.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sensor Readings'!$T$3:$T$322</c:f>
+              <c:f>'Sensor Readings'!$A$168:$A$223</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>20cm-25cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$B$223:$B$278</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3860.2</c:v>
+                  <c:v>1568.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3884.1</c:v>
+                  <c:v>1559.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3843.0</c:v>
+                  <c:v>1552.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3783.8</c:v>
+                  <c:v>1544.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3663.7</c:v>
+                  <c:v>1537.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3492.7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3212.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2840.3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2560.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2367.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2220.6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2100.3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2003.8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1927.1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1867.9</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1811.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1771.2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1739.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1709.9</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1686.6</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1666.2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1648.5</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1635.2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1621.4</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1610.4</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1600.6</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1590.6</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1584.8</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1576.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1570.2</c:v>
+                  <c:v>1532.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$A$223:$A$278</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>25cm-29</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$B$278:$B$322</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1532.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1528.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1524.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1520.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1519.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$A$278:$A$322</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1579,37 +1637,1546 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2052222360"/>
-        <c:axId val="2052219880"/>
+        <c:axId val="2075971864"/>
+        <c:axId val="2074145304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2052222360"/>
+        <c:axId val="2075971864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="0&quot; cm&quot;" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2052219880"/>
+        <c:crossAx val="2074145304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2052219880"/>
+        <c:axId val="2074145304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:numFmt formatCode="0&quot; cm&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2075971864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>0cm-5cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.127968825325406"/>
+                  <c:y val="-0.0748690613111562"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$H$3:$H$58</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3620.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3455.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3003.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2523.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2165.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1914.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$G$3:$G$58</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>5cm-10cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$H$58:$H$113</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1914.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1748.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1612.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1511.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1412.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1348.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$G$58:$G$113</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>10cm-15cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$H$113:$H$168</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1348.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1290.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1239.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1200.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1167.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1137.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$G$113:$G$168</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>15cm-20cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$H$168:$H$223</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1137.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1114.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1094.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1076.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1061.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1048.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$G$168:$G$223</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>20cm-25cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$H$223:$H$278</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1048.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1039.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1029.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1019.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1012.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1005.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$G$223:$G$278</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>25cm-29cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$H$278:$H$322</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1005.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>995.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>992.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>987.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$G$278:$G$322</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2069383960"/>
+        <c:axId val="2068942440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2069383960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2052222360"/>
+        <c:crossAx val="2068942440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2068942440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0&quot; cm&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2069383960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>"1cm-5cm"</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$N$14:$N$58</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3885.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3860.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3818.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3771.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3660.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$M$14:$M$58</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>5cm-10cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$N$58:$N$113</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3660.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3515.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3285.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2995.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2718.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2533.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$M$58:$M$113</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>10cm-15cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$N$113:$N$168</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2533.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2381.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2262.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2166.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2089.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2023.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$M$113:$M$168</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>15cm-20cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$N$168:$N$223</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2023.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1974.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1929.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1890.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1861.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1832.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$M$168:$M$223</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>20cm-25cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$N$223:$N$278</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1832.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1808.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1791.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1771.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1755.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1741.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$M$223:$M$278</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>25cm-29cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$N$278:$N$322</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1741.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1729.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1719.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1709.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1701.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$M$278:$M$322</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2079756488"/>
+        <c:axId val="2077458376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2079756488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2077458376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2077458376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0&quot; cm&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2079756488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1cm-5cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$T$14:$T$58</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3884.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3843.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3783.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3663.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3492.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$S$14:$S$58</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>5cm-10cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$T$58:$T$113</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3492.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3212.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2840.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2560.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2367.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2220.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$S$58:$S$113</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>10cm-15cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$T$113:$T$168</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2220.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2100.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2003.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1927.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1867.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1811.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$S$113:$S$168</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>15cm-20cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$T$168:$T$223</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1811.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1771.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1739.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1709.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1686.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1666.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$S$168:$S$223</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>20cm-25cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$T$223:$T$278</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1666.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1648.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1635.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1621.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1610.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1600.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$S$223:$S$278</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>25cm-29cm</c:v>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$T$278:$T$322</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1600.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1590.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1584.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1576.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1570.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sensor Readings'!$S$278:$S$322</c:f>
+              <c:numCache>
+                <c:formatCode>0" cm"</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2081587464"/>
+        <c:axId val="2081645208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2081587464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2081645208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2081645208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0&quot; cm&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2081587464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1635,21 +3202,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>333</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1676,9 +3245,120 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2027,8 +3707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H3" activeCellId="1" sqref="G3:G58 H3:H58"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A278" activeCellId="4" sqref="A58:XFD58 A113:XFD113 A168:XFD168 A223:XFD223 A278:XFD278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4257,80 +5937,80 @@
       <c r="U57" s="3"/>
       <c r="V57" s="3"/>
     </row>
-    <row r="58" spans="1:23">
-      <c r="A58" s="1">
+    <row r="58" spans="1:23" s="14" customFormat="1">
+      <c r="A58" s="11">
         <v>5</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="12">
         <f>AVERAGE(A59:A68)</f>
         <v>2334.5</v>
       </c>
-      <c r="C58" s="8">
+      <c r="C58" s="13">
         <f>STDEV(B59:B68)</f>
         <v>0.91893658347268148</v>
       </c>
-      <c r="D58" s="8">
+      <c r="D58" s="13">
         <f>MAX(B59:B68)-MIN(B59:B68)</f>
         <v>3</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="12">
         <f>AVERAGE(B59:B68)</f>
         <v>3294.8</v>
       </c>
-      <c r="G58" s="4">
+      <c r="G58" s="15">
         <v>5</v>
       </c>
-      <c r="H58" s="2">
+      <c r="H58" s="12">
         <f>AVERAGE(G59:G68)</f>
         <v>1914.5</v>
       </c>
-      <c r="I58" s="8">
+      <c r="I58" s="13">
         <f>STDEV(H59:H68)</f>
         <v>1.1352924243950935</v>
       </c>
-      <c r="J58" s="8">
+      <c r="J58" s="13">
         <f>MAX(H59:H68)-MIN(H59:H68)</f>
         <v>3</v>
       </c>
-      <c r="K58" s="2">
+      <c r="K58" s="12">
         <f>AVERAGE(H59:H68)</f>
         <v>3044.8</v>
       </c>
-      <c r="M58" s="4">
+      <c r="M58" s="15">
         <v>5</v>
       </c>
-      <c r="N58" s="2">
+      <c r="N58" s="12">
         <f>AVERAGE(M59:M68)</f>
         <v>3660.4</v>
       </c>
-      <c r="O58" s="8">
+      <c r="O58" s="13">
         <f>STDEV(N59:N68)</f>
         <v>1.2649110640673518</v>
       </c>
-      <c r="P58" s="8">
+      <c r="P58" s="13">
         <f>MAX(N59:N68)-MIN(N59:N68)</f>
         <v>5</v>
       </c>
-      <c r="Q58" s="2">
+      <c r="Q58" s="12">
         <f>AVERAGE(N59:N68)</f>
         <v>3101.4</v>
       </c>
-      <c r="S58" s="4">
+      <c r="S58" s="15">
         <v>5</v>
       </c>
-      <c r="T58" s="2">
+      <c r="T58" s="12">
         <f>AVERAGE(S59:S68)</f>
         <v>3492.7</v>
       </c>
-      <c r="U58" s="8">
+      <c r="U58" s="13">
         <f>STDEV(T59:T68)</f>
         <v>1.3498971154211057</v>
       </c>
-      <c r="V58" s="8">
+      <c r="V58" s="13">
         <f>MAX(T59:T68)-MIN(T59:T68)</f>
         <v>4</v>
       </c>
-      <c r="W58" s="2">
+      <c r="W58" s="12">
         <f>AVERAGE(T59:T68)</f>
         <v>3103.4</v>
       </c>
@@ -6397,80 +8077,80 @@
       <c r="U112" s="3"/>
       <c r="V112" s="3"/>
     </row>
-    <row r="113" spans="1:23">
-      <c r="A113" s="1">
+    <row r="113" spans="1:23" s="14" customFormat="1">
+      <c r="A113" s="11">
         <v>10</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B113" s="12">
         <f>AVERAGE(A114:A123)</f>
         <v>1823</v>
       </c>
-      <c r="C113" s="8">
+      <c r="C113" s="13">
         <f>STDEV(B114:B123)</f>
         <v>0.82327260234856459</v>
       </c>
-      <c r="D113" s="8">
+      <c r="D113" s="13">
         <f>MAX(B114:B123)-MIN(B114:B123)</f>
         <v>3</v>
       </c>
-      <c r="E113" s="2">
+      <c r="E113" s="12">
         <f>AVERAGE(B114:B123)</f>
         <v>3268.7</v>
       </c>
-      <c r="G113" s="4">
+      <c r="G113" s="15">
         <v>10</v>
       </c>
-      <c r="H113" s="2">
+      <c r="H113" s="12">
         <f>AVERAGE(G114:G123)</f>
         <v>1348.4</v>
       </c>
-      <c r="I113" s="8">
+      <c r="I113" s="13">
         <f>STDEV(H114:H123)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="J113" s="8">
+      <c r="J113" s="13">
         <f>MAX(H114:H123)-MIN(H114:H123)</f>
         <v>2</v>
       </c>
-      <c r="K113" s="2">
+      <c r="K113" s="12">
         <f>AVERAGE(H114:H123)</f>
         <v>3038</v>
       </c>
-      <c r="M113" s="4">
+      <c r="M113" s="15">
         <v>10</v>
       </c>
-      <c r="N113" s="2">
+      <c r="N113" s="12">
         <f>AVERAGE(M114:M123)</f>
         <v>2533</v>
       </c>
-      <c r="O113" s="8">
+      <c r="O113" s="13">
         <f>STDEV(N114:N123)</f>
         <v>1.699673171197595</v>
       </c>
-      <c r="P113" s="8">
+      <c r="P113" s="13">
         <f>MAX(N114:N123)-MIN(N114:N123)</f>
         <v>6</v>
       </c>
-      <c r="Q113" s="2">
+      <c r="Q113" s="12">
         <f>AVERAGE(N114:N123)</f>
         <v>3102</v>
       </c>
-      <c r="S113" s="4">
+      <c r="S113" s="15">
         <v>10</v>
       </c>
-      <c r="T113" s="2">
+      <c r="T113" s="12">
         <f>AVERAGE(S114:S123)</f>
         <v>2220.6</v>
       </c>
-      <c r="U113" s="8">
+      <c r="U113" s="13">
         <f>STDEV(T114:T123)</f>
         <v>1.5634719199411433</v>
       </c>
-      <c r="V113" s="8">
+      <c r="V113" s="13">
         <f>MAX(T114:T123)-MIN(T114:T123)</f>
         <v>6</v>
       </c>
-      <c r="W113" s="2">
+      <c r="W113" s="12">
         <f>AVERAGE(T114:T123)</f>
         <v>3101</v>
       </c>
@@ -8537,80 +10217,80 @@
       <c r="U167" s="3"/>
       <c r="V167" s="3"/>
     </row>
-    <row r="168" spans="1:23">
-      <c r="A168" s="1">
+    <row r="168" spans="1:23" s="14" customFormat="1">
+      <c r="A168" s="11">
         <v>15</v>
       </c>
-      <c r="B168" s="2">
+      <c r="B168" s="12">
         <f>AVERAGE(A169:A178)</f>
         <v>1642.2</v>
       </c>
-      <c r="C168" s="8">
+      <c r="C168" s="13">
         <f>STDEV(B169:B178)</f>
         <v>0.78881063774661553</v>
       </c>
-      <c r="D168" s="8">
+      <c r="D168" s="13">
         <f>MAX(B169:B178)-MIN(B169:B178)</f>
         <v>2</v>
       </c>
-      <c r="E168" s="2">
+      <c r="E168" s="12">
         <f>AVERAGE(B169:B178)</f>
         <v>3257.8</v>
       </c>
-      <c r="G168" s="4">
+      <c r="G168" s="15">
         <v>15</v>
       </c>
-      <c r="H168" s="2">
+      <c r="H168" s="12">
         <f>AVERAGE(G169:G178)</f>
         <v>1137.0999999999999</v>
       </c>
-      <c r="I168" s="8">
+      <c r="I168" s="13">
         <f>STDEV(H169:H178)</f>
         <v>1.1972189997378648</v>
       </c>
-      <c r="J168" s="8">
+      <c r="J168" s="13">
         <f>MAX(H169:H178)-MIN(H169:H178)</f>
         <v>3</v>
       </c>
-      <c r="K168" s="2">
+      <c r="K168" s="12">
         <f>AVERAGE(H169:H178)</f>
         <v>3038.9</v>
       </c>
-      <c r="M168" s="4">
+      <c r="M168" s="15">
         <v>15</v>
       </c>
-      <c r="N168" s="2">
+      <c r="N168" s="12">
         <f>AVERAGE(M169:M178)</f>
         <v>2023.4</v>
       </c>
-      <c r="O168" s="8">
+      <c r="O168" s="13">
         <f>STDEV(N169:N178)</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="P168" s="8">
+      <c r="P168" s="13">
         <f>MAX(N169:N178)-MIN(N169:N178)</f>
         <v>5</v>
       </c>
-      <c r="Q168" s="2">
+      <c r="Q168" s="12">
         <f>AVERAGE(N169:N178)</f>
         <v>3088</v>
       </c>
-      <c r="S168" s="4">
+      <c r="S168" s="15">
         <v>15</v>
       </c>
-      <c r="T168" s="2">
+      <c r="T168" s="12">
         <f>AVERAGE(S169:S178)</f>
         <v>1811.5</v>
       </c>
-      <c r="U168" s="8">
+      <c r="U168" s="13">
         <f>STDEV(T169:T178)</f>
         <v>1.3984117975602022</v>
       </c>
-      <c r="V168" s="8">
+      <c r="V168" s="13">
         <f>MAX(T169:T178)-MIN(T169:T178)</f>
         <v>5</v>
       </c>
-      <c r="W168" s="2">
+      <c r="W168" s="12">
         <f>AVERAGE(T169:T178)</f>
         <v>3100.2</v>
       </c>
@@ -10677,80 +12357,80 @@
       <c r="U222" s="3"/>
       <c r="V222" s="3"/>
     </row>
-    <row r="223" spans="1:23">
-      <c r="A223" s="1">
+    <row r="223" spans="1:23" s="14" customFormat="1">
+      <c r="A223" s="11">
         <v>20</v>
       </c>
-      <c r="B223" s="2">
+      <c r="B223" s="12">
         <f>AVERAGE(A224:A233)</f>
         <v>1568</v>
       </c>
-      <c r="C223" s="8">
+      <c r="C223" s="13">
         <f>STDEV(B224:B233)</f>
         <v>1.2292725943057186</v>
       </c>
-      <c r="D223" s="8">
+      <c r="D223" s="13">
         <f>MAX(B224:B233)-MIN(B224:B233)</f>
         <v>4</v>
       </c>
-      <c r="E223" s="2">
+      <c r="E223" s="12">
         <f>AVERAGE(B224:B233)</f>
         <v>3250.2</v>
       </c>
-      <c r="G223" s="4">
+      <c r="G223" s="15">
         <v>20</v>
       </c>
-      <c r="H223" s="2">
+      <c r="H223" s="12">
         <f>AVERAGE(G224:G233)</f>
         <v>1048.9000000000001</v>
       </c>
-      <c r="I223" s="8">
+      <c r="I223" s="13">
         <f>STDEV(H224:H233)</f>
         <v>1.1785113019775793</v>
       </c>
-      <c r="J223" s="8">
+      <c r="J223" s="13">
         <f>MAX(H224:H233)-MIN(H224:H233)</f>
         <v>3</v>
       </c>
-      <c r="K223" s="2">
+      <c r="K223" s="12">
         <f>AVERAGE(H224:H233)</f>
         <v>3035.5</v>
       </c>
-      <c r="M223" s="4">
+      <c r="M223" s="15">
         <v>20</v>
       </c>
-      <c r="N223" s="2">
+      <c r="N223" s="12">
         <f>AVERAGE(M224:M233)</f>
         <v>1832.7</v>
       </c>
-      <c r="O223" s="8">
+      <c r="O223" s="13">
         <f>STDEV(N224:N233)</f>
         <v>1.1972189997378648</v>
       </c>
-      <c r="P223" s="8">
+      <c r="P223" s="13">
         <f>MAX(N224:N233)-MIN(N224:N233)</f>
         <v>4</v>
       </c>
-      <c r="Q223" s="2">
+      <c r="Q223" s="12">
         <f>AVERAGE(N224:N233)</f>
         <v>3088.1</v>
       </c>
-      <c r="S223" s="4">
+      <c r="S223" s="15">
         <v>20</v>
       </c>
-      <c r="T223" s="2">
+      <c r="T223" s="12">
         <f>AVERAGE(S224:S233)</f>
         <v>1666.2</v>
       </c>
-      <c r="U223" s="8">
+      <c r="U223" s="13">
         <f>STDEV(T224:T233)</f>
         <v>1.3374935098492589</v>
       </c>
-      <c r="V223" s="8">
+      <c r="V223" s="13">
         <f>MAX(T224:T233)-MIN(T224:T233)</f>
         <v>5</v>
       </c>
-      <c r="W223" s="2">
+      <c r="W223" s="12">
         <f>AVERAGE(T224:T233)</f>
         <v>3098.3</v>
       </c>
@@ -12817,80 +14497,80 @@
       <c r="U277" s="3"/>
       <c r="V277" s="3"/>
     </row>
-    <row r="278" spans="1:23">
-      <c r="A278" s="1">
+    <row r="278" spans="1:23" s="14" customFormat="1">
+      <c r="A278" s="11">
         <v>25</v>
       </c>
-      <c r="B278" s="2">
+      <c r="B278" s="12">
         <f>AVERAGE(A279:A288)</f>
         <v>1532.6</v>
       </c>
-      <c r="C278" s="8">
+      <c r="C278" s="13">
         <f>STDEV(B279:B288)</f>
         <v>0.73786478737262196</v>
       </c>
-      <c r="D278" s="8">
+      <c r="D278" s="13">
         <f>MAX(B279:B288)-MIN(B279:B288)</f>
         <v>2</v>
       </c>
-      <c r="E278" s="2">
+      <c r="E278" s="12">
         <f>AVERAGE(B279:B288)</f>
         <v>3243.9</v>
       </c>
-      <c r="G278" s="4">
+      <c r="G278" s="15">
         <v>25</v>
       </c>
-      <c r="H278" s="2">
+      <c r="H278" s="12">
         <f>AVERAGE(G279:G288)</f>
         <v>1005.7</v>
       </c>
-      <c r="I278" s="8">
+      <c r="I278" s="13">
         <f>STDEV(H279:H288)</f>
         <v>0.84327404271156792</v>
       </c>
-      <c r="J278" s="8">
+      <c r="J278" s="13">
         <f>MAX(H279:H288)-MIN(H279:H288)</f>
         <v>3</v>
       </c>
-      <c r="K278" s="2">
+      <c r="K278" s="12">
         <f>AVERAGE(H279:H288)</f>
         <v>3033.6</v>
       </c>
-      <c r="M278" s="4">
+      <c r="M278" s="15">
         <v>25</v>
       </c>
-      <c r="N278" s="2">
+      <c r="N278" s="12">
         <f>AVERAGE(M279:M288)</f>
         <v>1741.5</v>
       </c>
-      <c r="O278" s="8">
+      <c r="O278" s="13">
         <f>STDEV(N279:N288)</f>
         <v>0.94868329805051377</v>
       </c>
-      <c r="P278" s="8">
+      <c r="P278" s="13">
         <f>MAX(N279:N288)-MIN(N279:N288)</f>
         <v>3</v>
       </c>
-      <c r="Q278" s="2">
+      <c r="Q278" s="12">
         <f>AVERAGE(N279:N288)</f>
         <v>3097.3</v>
       </c>
-      <c r="S278" s="4">
+      <c r="S278" s="15">
         <v>25</v>
       </c>
-      <c r="T278" s="2">
+      <c r="T278" s="12">
         <f>AVERAGE(S279:S288)</f>
         <v>1600.6</v>
       </c>
-      <c r="U278" s="8">
+      <c r="U278" s="13">
         <f>STDEV(T279:T288)</f>
         <v>1.0593499054713802</v>
       </c>
-      <c r="V278" s="8">
+      <c r="V278" s="13">
         <f>MAX(T279:T288)-MIN(T279:T288)</f>
         <v>3</v>
       </c>
-      <c r="W278" s="2">
+      <c r="W278" s="12">
         <f>AVERAGE(T279:T288)</f>
         <v>3097.3</v>
       </c>
@@ -14935,7 +16615,6 @@
     <mergeCell ref="G1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -14960,4 +16639,76 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>